<commit_message>
Atualizado por script em 20-12-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/serbia_super-liga_2023-2024.xlsx
+++ b/2023/serbia_super-liga_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V143"/>
+  <dimension ref="A1:V144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2137,7 +2137,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>TSC</t>
+          <t>Vozdovac</t>
         </is>
       </c>
       <c r="G19" t="n">
@@ -2145,14 +2145,14 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Radnicki 1923</t>
+          <t>Radnik</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="n">
-        <v>1.33</v>
+        <v>3.21</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
@@ -2160,15 +2160,15 @@
         </is>
       </c>
       <c r="L19" t="n">
-        <v>1.47</v>
+        <v>2.12</v>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>12/08/2023 16:58</t>
+          <t>12/08/2023 18:54</t>
         </is>
       </c>
       <c r="N19" t="n">
-        <v>4.58</v>
+        <v>3.12</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -2176,15 +2176,15 @@
         </is>
       </c>
       <c r="P19" t="n">
-        <v>4.35</v>
+        <v>3.16</v>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>12/08/2023 18:50</t>
+          <t>12/08/2023 18:54</t>
         </is>
       </c>
       <c r="R19" t="n">
-        <v>7</v>
+        <v>2.11</v>
       </c>
       <c r="S19" t="inlineStr">
         <is>
@@ -2192,16 +2192,16 @@
         </is>
       </c>
       <c r="T19" t="n">
-        <v>6.26</v>
+        <v>3.53</v>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>12/08/2023 18:50</t>
+          <t>12/08/2023 18:54</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/serbia/super-liga/tsc-backa-topola-radnicki-1923/vVDe3xcd/</t>
+          <t>https://www.betexplorer.com/football/serbia/super-liga/fk-vozdovac-radnik-surdulica/WOOL9vKS/</t>
         </is>
       </c>
     </row>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Vozdovac</t>
+          <t>TSC</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -2237,14 +2237,14 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Radnik</t>
+          <t>Radnicki 1923</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>3.21</v>
+        <v>1.33</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
@@ -2252,15 +2252,15 @@
         </is>
       </c>
       <c r="L20" t="n">
-        <v>2.12</v>
+        <v>1.47</v>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>12/08/2023 18:54</t>
+          <t>12/08/2023 16:58</t>
         </is>
       </c>
       <c r="N20" t="n">
-        <v>3.12</v>
+        <v>4.58</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -2268,15 +2268,15 @@
         </is>
       </c>
       <c r="P20" t="n">
-        <v>3.16</v>
+        <v>4.35</v>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>12/08/2023 18:54</t>
+          <t>12/08/2023 18:50</t>
         </is>
       </c>
       <c r="R20" t="n">
-        <v>2.11</v>
+        <v>7</v>
       </c>
       <c r="S20" t="inlineStr">
         <is>
@@ -2284,16 +2284,16 @@
         </is>
       </c>
       <c r="T20" t="n">
-        <v>3.53</v>
+        <v>6.26</v>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>12/08/2023 18:54</t>
+          <t>12/08/2023 18:50</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/serbia/super-liga/fk-vozdovac-radnik-surdulica/WOOL9vKS/</t>
+          <t>https://www.betexplorer.com/football/serbia/super-liga/tsc-backa-topola-radnicki-1923/vVDe3xcd/</t>
         </is>
       </c>
     </row>
@@ -3885,22 +3885,22 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Cukaricki</t>
+          <t>Sp. Subotica</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Radnik</t>
+          <t>Napredak</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J38" t="n">
-        <v>1.44</v>
+        <v>1.93</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
@@ -3908,15 +3908,15 @@
         </is>
       </c>
       <c r="L38" t="n">
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>27/08/2023 19:25</t>
+          <t>27/08/2023 19:29</t>
         </is>
       </c>
       <c r="N38" t="n">
-        <v>4.05</v>
+        <v>3.1</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3924,15 +3924,15 @@
         </is>
       </c>
       <c r="P38" t="n">
-        <v>4.26</v>
+        <v>3.23</v>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>27/08/2023 19:25</t>
+          <t>27/08/2023 19:29</t>
         </is>
       </c>
       <c r="R38" t="n">
-        <v>5.74</v>
+        <v>3.63</v>
       </c>
       <c r="S38" t="inlineStr">
         <is>
@@ -3940,16 +3940,16 @@
         </is>
       </c>
       <c r="T38" t="n">
-        <v>8.359999999999999</v>
+        <v>3.82</v>
       </c>
       <c r="U38" t="inlineStr">
         <is>
-          <t>27/08/2023 19:25</t>
+          <t>27/08/2023 19:29</t>
         </is>
       </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/serbia/super-liga/cukaricki-radnik-surdulica/Iu9Yyc3L/</t>
+          <t>https://www.betexplorer.com/football/serbia/super-liga/spartak-subotica-napredak/rNGLvaJ2/</t>
         </is>
       </c>
     </row>
@@ -3977,22 +3977,22 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Sp. Subotica</t>
+          <t>Cukaricki</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Napredak</t>
+          <t>Radnik</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>1.93</v>
+        <v>1.44</v>
       </c>
       <c r="K39" t="inlineStr">
         <is>
@@ -4000,15 +4000,15 @@
         </is>
       </c>
       <c r="L39" t="n">
-        <v>2</v>
+        <v>1.4</v>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>27/08/2023 19:29</t>
+          <t>27/08/2023 19:25</t>
         </is>
       </c>
       <c r="N39" t="n">
-        <v>3.1</v>
+        <v>4.05</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -4016,15 +4016,15 @@
         </is>
       </c>
       <c r="P39" t="n">
-        <v>3.23</v>
+        <v>4.26</v>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>27/08/2023 19:29</t>
+          <t>27/08/2023 19:25</t>
         </is>
       </c>
       <c r="R39" t="n">
-        <v>3.63</v>
+        <v>5.74</v>
       </c>
       <c r="S39" t="inlineStr">
         <is>
@@ -4032,16 +4032,16 @@
         </is>
       </c>
       <c r="T39" t="n">
-        <v>3.82</v>
+        <v>8.359999999999999</v>
       </c>
       <c r="U39" t="inlineStr">
         <is>
-          <t>27/08/2023 19:29</t>
+          <t>27/08/2023 19:25</t>
         </is>
       </c>
       <c r="V39" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/serbia/super-liga/spartak-subotica-napredak/rNGLvaJ2/</t>
+          <t>https://www.betexplorer.com/football/serbia/super-liga/cukaricki-radnik-surdulica/Iu9Yyc3L/</t>
         </is>
       </c>
     </row>
@@ -4989,22 +4989,22 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>TSC</t>
+          <t>Vozdovac</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Zeleznicar Pancevo</t>
+          <t>Mladost</t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J50" t="n">
-        <v>1.21</v>
+        <v>2.07</v>
       </c>
       <c r="K50" t="inlineStr">
         <is>
@@ -5012,7 +5012,7 @@
         </is>
       </c>
       <c r="L50" t="n">
-        <v>1.33</v>
+        <v>1.83</v>
       </c>
       <c r="M50" t="inlineStr">
         <is>
@@ -5020,7 +5020,7 @@
         </is>
       </c>
       <c r="N50" t="n">
-        <v>5.61</v>
+        <v>3.13</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -5028,7 +5028,7 @@
         </is>
       </c>
       <c r="P50" t="n">
-        <v>4.42</v>
+        <v>3.58</v>
       </c>
       <c r="Q50" t="inlineStr">
         <is>
@@ -5036,7 +5036,7 @@
         </is>
       </c>
       <c r="R50" t="n">
-        <v>9.23</v>
+        <v>3.2</v>
       </c>
       <c r="S50" t="inlineStr">
         <is>
@@ -5044,7 +5044,7 @@
         </is>
       </c>
       <c r="T50" t="n">
-        <v>10.82</v>
+        <v>4.06</v>
       </c>
       <c r="U50" t="inlineStr">
         <is>
@@ -5053,7 +5053,7 @@
       </c>
       <c r="V50" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/serbia/super-liga/tsc-backa-topola-zeleznicar-pancevo/xOIdSqWO/</t>
+          <t>https://www.betexplorer.com/football/serbia/super-liga/fk-vozdovac-mladost-lucani/25QqVon6/</t>
         </is>
       </c>
     </row>
@@ -5081,22 +5081,22 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Vozdovac</t>
+          <t>TSC</t>
         </is>
       </c>
       <c r="G51" t="n">
+        <v>6</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Zeleznicar Pancevo</t>
+        </is>
+      </c>
+      <c r="I51" t="n">
         <v>3</v>
       </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>Mladost</t>
-        </is>
-      </c>
-      <c r="I51" t="n">
-        <v>1</v>
-      </c>
       <c r="J51" t="n">
-        <v>2.07</v>
+        <v>1.21</v>
       </c>
       <c r="K51" t="inlineStr">
         <is>
@@ -5104,7 +5104,7 @@
         </is>
       </c>
       <c r="L51" t="n">
-        <v>1.83</v>
+        <v>1.33</v>
       </c>
       <c r="M51" t="inlineStr">
         <is>
@@ -5112,7 +5112,7 @@
         </is>
       </c>
       <c r="N51" t="n">
-        <v>3.13</v>
+        <v>5.61</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -5120,7 +5120,7 @@
         </is>
       </c>
       <c r="P51" t="n">
-        <v>3.58</v>
+        <v>4.42</v>
       </c>
       <c r="Q51" t="inlineStr">
         <is>
@@ -5128,7 +5128,7 @@
         </is>
       </c>
       <c r="R51" t="n">
-        <v>3.2</v>
+        <v>9.23</v>
       </c>
       <c r="S51" t="inlineStr">
         <is>
@@ -5136,7 +5136,7 @@
         </is>
       </c>
       <c r="T51" t="n">
-        <v>4.06</v>
+        <v>10.82</v>
       </c>
       <c r="U51" t="inlineStr">
         <is>
@@ -5145,7 +5145,7 @@
       </c>
       <c r="V51" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/serbia/super-liga/fk-vozdovac-mladost-lucani/25QqVon6/</t>
+          <t>https://www.betexplorer.com/football/serbia/super-liga/tsc-backa-topola-zeleznicar-pancevo/xOIdSqWO/</t>
         </is>
       </c>
     </row>
@@ -8117,22 +8117,22 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Mladost</t>
+          <t>Vojvodina</t>
         </is>
       </c>
       <c r="G84" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Radnicki Nis</t>
+          <t>Radnik</t>
         </is>
       </c>
       <c r="I84" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J84" t="n">
-        <v>1.78</v>
+        <v>1.61</v>
       </c>
       <c r="K84" t="inlineStr">
         <is>
@@ -8140,15 +8140,15 @@
         </is>
       </c>
       <c r="L84" t="n">
-        <v>2.87</v>
+        <v>1.34</v>
       </c>
       <c r="M84" t="inlineStr">
         <is>
-          <t>22/10/2023 17:59</t>
+          <t>22/10/2023 17:51</t>
         </is>
       </c>
       <c r="N84" t="n">
-        <v>3.36</v>
+        <v>3.58</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
@@ -8156,15 +8156,15 @@
         </is>
       </c>
       <c r="P84" t="n">
-        <v>3.13</v>
+        <v>4.63</v>
       </c>
       <c r="Q84" t="inlineStr">
         <is>
-          <t>22/10/2023 17:59</t>
+          <t>22/10/2023 17:51</t>
         </is>
       </c>
       <c r="R84" t="n">
-        <v>4.07</v>
+        <v>4.69</v>
       </c>
       <c r="S84" t="inlineStr">
         <is>
@@ -8172,16 +8172,16 @@
         </is>
       </c>
       <c r="T84" t="n">
-        <v>2.48</v>
+        <v>9.609999999999999</v>
       </c>
       <c r="U84" t="inlineStr">
         <is>
-          <t>22/10/2023 17:59</t>
+          <t>22/10/2023 17:51</t>
         </is>
       </c>
       <c r="V84" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/serbia/super-liga/mladost-lucani-radnicki-nis/0GjCx957/</t>
+          <t>https://www.betexplorer.com/football/serbia/super-liga/vojvodina-radnik-surdulica/Ctudti6r/</t>
         </is>
       </c>
     </row>
@@ -8209,22 +8209,22 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Vojvodina</t>
+          <t>Mladost</t>
         </is>
       </c>
       <c r="G85" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Radnik</t>
+          <t>Radnicki Nis</t>
         </is>
       </c>
       <c r="I85" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J85" t="n">
-        <v>1.61</v>
+        <v>1.78</v>
       </c>
       <c r="K85" t="inlineStr">
         <is>
@@ -8232,15 +8232,15 @@
         </is>
       </c>
       <c r="L85" t="n">
-        <v>1.34</v>
+        <v>2.87</v>
       </c>
       <c r="M85" t="inlineStr">
         <is>
-          <t>22/10/2023 17:51</t>
+          <t>22/10/2023 17:59</t>
         </is>
       </c>
       <c r="N85" t="n">
-        <v>3.58</v>
+        <v>3.36</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
@@ -8248,15 +8248,15 @@
         </is>
       </c>
       <c r="P85" t="n">
-        <v>4.63</v>
+        <v>3.13</v>
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>22/10/2023 17:51</t>
+          <t>22/10/2023 17:59</t>
         </is>
       </c>
       <c r="R85" t="n">
-        <v>4.69</v>
+        <v>4.07</v>
       </c>
       <c r="S85" t="inlineStr">
         <is>
@@ -8264,16 +8264,16 @@
         </is>
       </c>
       <c r="T85" t="n">
-        <v>9.609999999999999</v>
+        <v>2.48</v>
       </c>
       <c r="U85" t="inlineStr">
         <is>
-          <t>22/10/2023 17:51</t>
+          <t>22/10/2023 17:59</t>
         </is>
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/serbia/super-liga/vojvodina-radnik-surdulica/Ctudti6r/</t>
+          <t>https://www.betexplorer.com/football/serbia/super-liga/mladost-lucani-radnicki-nis/0GjCx957/</t>
         </is>
       </c>
     </row>
@@ -8669,7 +8669,7 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Radnicki Nis</t>
+          <t>IMT Novi Beograd</t>
         </is>
       </c>
       <c r="G90" t="n">
@@ -8677,14 +8677,14 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Sp. Subotica</t>
+          <t>Crvena zvezda</t>
         </is>
       </c>
       <c r="I90" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J90" t="n">
-        <v>1.7</v>
+        <v>8.15</v>
       </c>
       <c r="K90" t="inlineStr">
         <is>
@@ -8692,15 +8692,15 @@
         </is>
       </c>
       <c r="L90" t="n">
-        <v>1.66</v>
+        <v>24.2</v>
       </c>
       <c r="M90" t="inlineStr">
         <is>
-          <t>28/10/2023 18:23</t>
+          <t>28/10/2023 18:29</t>
         </is>
       </c>
       <c r="N90" t="n">
-        <v>3.42</v>
+        <v>5.6</v>
       </c>
       <c r="O90" t="inlineStr">
         <is>
@@ -8708,15 +8708,15 @@
         </is>
       </c>
       <c r="P90" t="n">
-        <v>3.65</v>
+        <v>9.529999999999999</v>
       </c>
       <c r="Q90" t="inlineStr">
         <is>
-          <t>28/10/2023 18:23</t>
+          <t>28/10/2023 18:29</t>
         </is>
       </c>
       <c r="R90" t="n">
-        <v>4.23</v>
+        <v>1.23</v>
       </c>
       <c r="S90" t="inlineStr">
         <is>
@@ -8724,16 +8724,16 @@
         </is>
       </c>
       <c r="T90" t="n">
-        <v>5.08</v>
+        <v>1.09</v>
       </c>
       <c r="U90" t="inlineStr">
         <is>
-          <t>28/10/2023 18:23</t>
+          <t>28/10/2023 18:21</t>
         </is>
       </c>
       <c r="V90" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/serbia/super-liga/radnicki-nis-spartak-subotica/2qDshl5f/</t>
+          <t>https://www.betexplorer.com/football/serbia/super-liga/imt-novi-beograd-crvena-zvezda/SjAgknkD/</t>
         </is>
       </c>
     </row>
@@ -8761,7 +8761,7 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>IMT Novi Beograd</t>
+          <t>Radnicki Nis</t>
         </is>
       </c>
       <c r="G91" t="n">
@@ -8769,14 +8769,14 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>Crvena zvezda</t>
+          <t>Sp. Subotica</t>
         </is>
       </c>
       <c r="I91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J91" t="n">
-        <v>8.15</v>
+        <v>1.7</v>
       </c>
       <c r="K91" t="inlineStr">
         <is>
@@ -8784,15 +8784,15 @@
         </is>
       </c>
       <c r="L91" t="n">
-        <v>24.2</v>
+        <v>1.66</v>
       </c>
       <c r="M91" t="inlineStr">
         <is>
-          <t>28/10/2023 18:29</t>
+          <t>28/10/2023 18:23</t>
         </is>
       </c>
       <c r="N91" t="n">
-        <v>5.6</v>
+        <v>3.42</v>
       </c>
       <c r="O91" t="inlineStr">
         <is>
@@ -8800,15 +8800,15 @@
         </is>
       </c>
       <c r="P91" t="n">
-        <v>9.529999999999999</v>
+        <v>3.65</v>
       </c>
       <c r="Q91" t="inlineStr">
         <is>
-          <t>28/10/2023 18:29</t>
+          <t>28/10/2023 18:23</t>
         </is>
       </c>
       <c r="R91" t="n">
-        <v>1.23</v>
+        <v>4.23</v>
       </c>
       <c r="S91" t="inlineStr">
         <is>
@@ -8816,16 +8816,16 @@
         </is>
       </c>
       <c r="T91" t="n">
-        <v>1.09</v>
+        <v>5.08</v>
       </c>
       <c r="U91" t="inlineStr">
         <is>
-          <t>28/10/2023 18:21</t>
+          <t>28/10/2023 18:23</t>
         </is>
       </c>
       <c r="V91" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/serbia/super-liga/imt-novi-beograd-crvena-zvezda/SjAgknkD/</t>
+          <t>https://www.betexplorer.com/football/serbia/super-liga/radnicki-nis-spartak-subotica/2qDshl5f/</t>
         </is>
       </c>
     </row>
@@ -11613,22 +11613,22 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>Partizan</t>
+          <t>Mladost</t>
         </is>
       </c>
       <c r="G122" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>Vojvodina</t>
+          <t>Zeleznicar Pancevo</t>
         </is>
       </c>
       <c r="I122" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J122" t="n">
-        <v>1.5</v>
+        <v>2.32</v>
       </c>
       <c r="K122" t="inlineStr">
         <is>
@@ -11636,15 +11636,15 @@
         </is>
       </c>
       <c r="L122" t="n">
-        <v>1.51</v>
+        <v>2.14</v>
       </c>
       <c r="M122" t="inlineStr">
         <is>
-          <t>02/12/2023 15:26</t>
+          <t>02/12/2023 15:03</t>
         </is>
       </c>
       <c r="N122" t="n">
-        <v>4.01</v>
+        <v>2.97</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -11652,15 +11652,15 @@
         </is>
       </c>
       <c r="P122" t="n">
-        <v>3.71</v>
+        <v>3.24</v>
       </c>
       <c r="Q122" t="inlineStr">
         <is>
-          <t>02/12/2023 15:26</t>
+          <t>02/12/2023 15:03</t>
         </is>
       </c>
       <c r="R122" t="n">
-        <v>5.3</v>
+        <v>2.94</v>
       </c>
       <c r="S122" t="inlineStr">
         <is>
@@ -11668,16 +11668,16 @@
         </is>
       </c>
       <c r="T122" t="n">
-        <v>7.24</v>
+        <v>3.38</v>
       </c>
       <c r="U122" t="inlineStr">
         <is>
-          <t>02/12/2023 15:26</t>
+          <t>02/12/2023 15:03</t>
         </is>
       </c>
       <c r="V122" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/serbia/super-liga/partizan-vojvodina/tUjxVN25/</t>
+          <t>https://www.betexplorer.com/football/serbia/super-liga/mladost-lucani-zeleznicar-pancevo/zka4Yd9c/</t>
         </is>
       </c>
     </row>
@@ -11705,22 +11705,22 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>Mladost</t>
+          <t>Partizan</t>
         </is>
       </c>
       <c r="G123" t="n">
+        <v>3</v>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>Vojvodina</t>
+        </is>
+      </c>
+      <c r="I123" t="n">
         <v>1</v>
       </c>
-      <c r="H123" t="inlineStr">
-        <is>
-          <t>Zeleznicar Pancevo</t>
-        </is>
-      </c>
-      <c r="I123" t="n">
-        <v>0</v>
-      </c>
       <c r="J123" t="n">
-        <v>2.32</v>
+        <v>1.5</v>
       </c>
       <c r="K123" t="inlineStr">
         <is>
@@ -11728,15 +11728,15 @@
         </is>
       </c>
       <c r="L123" t="n">
-        <v>2.14</v>
+        <v>1.51</v>
       </c>
       <c r="M123" t="inlineStr">
         <is>
-          <t>02/12/2023 15:03</t>
+          <t>02/12/2023 15:26</t>
         </is>
       </c>
       <c r="N123" t="n">
-        <v>2.97</v>
+        <v>4.01</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -11744,15 +11744,15 @@
         </is>
       </c>
       <c r="P123" t="n">
-        <v>3.24</v>
+        <v>3.71</v>
       </c>
       <c r="Q123" t="inlineStr">
         <is>
-          <t>02/12/2023 15:03</t>
+          <t>02/12/2023 15:26</t>
         </is>
       </c>
       <c r="R123" t="n">
-        <v>2.94</v>
+        <v>5.3</v>
       </c>
       <c r="S123" t="inlineStr">
         <is>
@@ -11760,16 +11760,16 @@
         </is>
       </c>
       <c r="T123" t="n">
-        <v>3.38</v>
+        <v>7.24</v>
       </c>
       <c r="U123" t="inlineStr">
         <is>
-          <t>02/12/2023 15:03</t>
+          <t>02/12/2023 15:26</t>
         </is>
       </c>
       <c r="V123" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/serbia/super-liga/mladost-lucani-zeleznicar-pancevo/zka4Yd9c/</t>
+          <t>https://www.betexplorer.com/football/serbia/super-liga/partizan-vojvodina/tUjxVN25/</t>
         </is>
       </c>
     </row>
@@ -13610,6 +13610,98 @@
       <c r="V143" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/serbia/super-liga/cukaricki-imt-novi-beograd/QcGbrYxM/</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>serbia</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>super-liga</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E144" s="2" t="n">
+        <v>45280.54166666666</v>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>Radnicki 1923</t>
+        </is>
+      </c>
+      <c r="G144" t="n">
+        <v>1</v>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>Radnik</t>
+        </is>
+      </c>
+      <c r="I144" t="n">
+        <v>0</v>
+      </c>
+      <c r="J144" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>25/09/2023 03:12</t>
+        </is>
+      </c>
+      <c r="L144" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="M144" t="inlineStr">
+        <is>
+          <t>20/12/2023 12:53</t>
+        </is>
+      </c>
+      <c r="N144" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="O144" t="inlineStr">
+        <is>
+          <t>25/09/2023 03:12</t>
+        </is>
+      </c>
+      <c r="P144" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="Q144" t="inlineStr">
+        <is>
+          <t>20/12/2023 12:53</t>
+        </is>
+      </c>
+      <c r="R144" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="S144" t="inlineStr">
+        <is>
+          <t>25/09/2023 03:12</t>
+        </is>
+      </c>
+      <c r="T144" t="n">
+        <v>6.57</v>
+      </c>
+      <c r="U144" t="inlineStr">
+        <is>
+          <t>20/12/2023 12:53</t>
+        </is>
+      </c>
+      <c r="V144" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/serbia/super-liga/radnicki-1923-radnik-surdulica/4CHCgMUN/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 21-12-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/serbia_super-liga_2023-2024.xlsx
+++ b/2023/serbia_super-liga_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V145"/>
+  <dimension ref="A1:V146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8117,22 +8117,22 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Mladost</t>
+          <t>Vojvodina</t>
         </is>
       </c>
       <c r="G84" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Radnicki Nis</t>
+          <t>Radnik</t>
         </is>
       </c>
       <c r="I84" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J84" t="n">
-        <v>1.78</v>
+        <v>1.61</v>
       </c>
       <c r="K84" t="inlineStr">
         <is>
@@ -8140,15 +8140,15 @@
         </is>
       </c>
       <c r="L84" t="n">
-        <v>2.87</v>
+        <v>1.34</v>
       </c>
       <c r="M84" t="inlineStr">
         <is>
-          <t>22/10/2023 17:59</t>
+          <t>22/10/2023 17:51</t>
         </is>
       </c>
       <c r="N84" t="n">
-        <v>3.36</v>
+        <v>3.58</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
@@ -8156,15 +8156,15 @@
         </is>
       </c>
       <c r="P84" t="n">
-        <v>3.13</v>
+        <v>4.63</v>
       </c>
       <c r="Q84" t="inlineStr">
         <is>
-          <t>22/10/2023 17:59</t>
+          <t>22/10/2023 17:51</t>
         </is>
       </c>
       <c r="R84" t="n">
-        <v>4.07</v>
+        <v>4.69</v>
       </c>
       <c r="S84" t="inlineStr">
         <is>
@@ -8172,16 +8172,16 @@
         </is>
       </c>
       <c r="T84" t="n">
-        <v>2.48</v>
+        <v>9.609999999999999</v>
       </c>
       <c r="U84" t="inlineStr">
         <is>
-          <t>22/10/2023 17:59</t>
+          <t>22/10/2023 17:51</t>
         </is>
       </c>
       <c r="V84" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/serbia/super-liga/mladost-lucani-radnicki-nis/0GjCx957/</t>
+          <t>https://www.betexplorer.com/football/serbia/super-liga/vojvodina-radnik-surdulica/Ctudti6r/</t>
         </is>
       </c>
     </row>
@@ -8209,22 +8209,22 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Vojvodina</t>
+          <t>Mladost</t>
         </is>
       </c>
       <c r="G85" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Radnik</t>
+          <t>Radnicki Nis</t>
         </is>
       </c>
       <c r="I85" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J85" t="n">
-        <v>1.61</v>
+        <v>1.78</v>
       </c>
       <c r="K85" t="inlineStr">
         <is>
@@ -8232,15 +8232,15 @@
         </is>
       </c>
       <c r="L85" t="n">
-        <v>1.34</v>
+        <v>2.87</v>
       </c>
       <c r="M85" t="inlineStr">
         <is>
-          <t>22/10/2023 17:51</t>
+          <t>22/10/2023 17:59</t>
         </is>
       </c>
       <c r="N85" t="n">
-        <v>3.58</v>
+        <v>3.36</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
@@ -8248,15 +8248,15 @@
         </is>
       </c>
       <c r="P85" t="n">
-        <v>4.63</v>
+        <v>3.13</v>
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>22/10/2023 17:51</t>
+          <t>22/10/2023 17:59</t>
         </is>
       </c>
       <c r="R85" t="n">
-        <v>4.69</v>
+        <v>4.07</v>
       </c>
       <c r="S85" t="inlineStr">
         <is>
@@ -8264,16 +8264,16 @@
         </is>
       </c>
       <c r="T85" t="n">
-        <v>9.609999999999999</v>
+        <v>2.48</v>
       </c>
       <c r="U85" t="inlineStr">
         <is>
-          <t>22/10/2023 17:51</t>
+          <t>22/10/2023 17:59</t>
         </is>
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/serbia/super-liga/vojvodina-radnik-surdulica/Ctudti6r/</t>
+          <t>https://www.betexplorer.com/football/serbia/super-liga/mladost-lucani-radnicki-nis/0GjCx957/</t>
         </is>
       </c>
     </row>
@@ -8669,7 +8669,7 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Radnicki Nis</t>
+          <t>IMT Novi Beograd</t>
         </is>
       </c>
       <c r="G90" t="n">
@@ -8677,14 +8677,14 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Sp. Subotica</t>
+          <t>Crvena zvezda</t>
         </is>
       </c>
       <c r="I90" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J90" t="n">
-        <v>1.7</v>
+        <v>8.15</v>
       </c>
       <c r="K90" t="inlineStr">
         <is>
@@ -8692,15 +8692,15 @@
         </is>
       </c>
       <c r="L90" t="n">
-        <v>1.66</v>
+        <v>24.2</v>
       </c>
       <c r="M90" t="inlineStr">
         <is>
-          <t>28/10/2023 18:23</t>
+          <t>28/10/2023 18:29</t>
         </is>
       </c>
       <c r="N90" t="n">
-        <v>3.42</v>
+        <v>5.6</v>
       </c>
       <c r="O90" t="inlineStr">
         <is>
@@ -8708,15 +8708,15 @@
         </is>
       </c>
       <c r="P90" t="n">
-        <v>3.65</v>
+        <v>9.529999999999999</v>
       </c>
       <c r="Q90" t="inlineStr">
         <is>
-          <t>28/10/2023 18:23</t>
+          <t>28/10/2023 18:29</t>
         </is>
       </c>
       <c r="R90" t="n">
-        <v>4.23</v>
+        <v>1.23</v>
       </c>
       <c r="S90" t="inlineStr">
         <is>
@@ -8724,16 +8724,16 @@
         </is>
       </c>
       <c r="T90" t="n">
-        <v>5.08</v>
+        <v>1.09</v>
       </c>
       <c r="U90" t="inlineStr">
         <is>
-          <t>28/10/2023 18:23</t>
+          <t>28/10/2023 18:21</t>
         </is>
       </c>
       <c r="V90" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/serbia/super-liga/radnicki-nis-spartak-subotica/2qDshl5f/</t>
+          <t>https://www.betexplorer.com/football/serbia/super-liga/imt-novi-beograd-crvena-zvezda/SjAgknkD/</t>
         </is>
       </c>
     </row>
@@ -8761,7 +8761,7 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>IMT Novi Beograd</t>
+          <t>Radnicki Nis</t>
         </is>
       </c>
       <c r="G91" t="n">
@@ -8769,14 +8769,14 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>Crvena zvezda</t>
+          <t>Sp. Subotica</t>
         </is>
       </c>
       <c r="I91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J91" t="n">
-        <v>8.15</v>
+        <v>1.7</v>
       </c>
       <c r="K91" t="inlineStr">
         <is>
@@ -8784,15 +8784,15 @@
         </is>
       </c>
       <c r="L91" t="n">
-        <v>24.2</v>
+        <v>1.66</v>
       </c>
       <c r="M91" t="inlineStr">
         <is>
-          <t>28/10/2023 18:29</t>
+          <t>28/10/2023 18:23</t>
         </is>
       </c>
       <c r="N91" t="n">
-        <v>5.6</v>
+        <v>3.42</v>
       </c>
       <c r="O91" t="inlineStr">
         <is>
@@ -8800,15 +8800,15 @@
         </is>
       </c>
       <c r="P91" t="n">
-        <v>9.529999999999999</v>
+        <v>3.65</v>
       </c>
       <c r="Q91" t="inlineStr">
         <is>
-          <t>28/10/2023 18:29</t>
+          <t>28/10/2023 18:23</t>
         </is>
       </c>
       <c r="R91" t="n">
-        <v>1.23</v>
+        <v>4.23</v>
       </c>
       <c r="S91" t="inlineStr">
         <is>
@@ -8816,16 +8816,16 @@
         </is>
       </c>
       <c r="T91" t="n">
-        <v>1.09</v>
+        <v>5.08</v>
       </c>
       <c r="U91" t="inlineStr">
         <is>
-          <t>28/10/2023 18:21</t>
+          <t>28/10/2023 18:23</t>
         </is>
       </c>
       <c r="V91" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/serbia/super-liga/imt-novi-beograd-crvena-zvezda/SjAgknkD/</t>
+          <t>https://www.betexplorer.com/football/serbia/super-liga/radnicki-nis-spartak-subotica/2qDshl5f/</t>
         </is>
       </c>
     </row>
@@ -13794,6 +13794,98 @@
       <c r="V145" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/serbia/super-liga/partizan-crvena-zvezda/WbJ4er0B/</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>serbia</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>super-liga</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E146" s="2" t="n">
+        <v>45281.625</v>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Novi Pazar</t>
+        </is>
+      </c>
+      <c r="G146" t="n">
+        <v>0</v>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>Sp. Subotica</t>
+        </is>
+      </c>
+      <c r="I146" t="n">
+        <v>1</v>
+      </c>
+      <c r="J146" t="n">
+        <v>2</v>
+      </c>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>26/09/2023 13:42</t>
+        </is>
+      </c>
+      <c r="L146" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="M146" t="inlineStr">
+        <is>
+          <t>21/12/2023 14:36</t>
+        </is>
+      </c>
+      <c r="N146" t="n">
+        <v>3.14</v>
+      </c>
+      <c r="O146" t="inlineStr">
+        <is>
+          <t>26/09/2023 13:42</t>
+        </is>
+      </c>
+      <c r="P146" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="Q146" t="inlineStr">
+        <is>
+          <t>21/12/2023 14:36</t>
+        </is>
+      </c>
+      <c r="R146" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="S146" t="inlineStr">
+        <is>
+          <t>26/09/2023 13:42</t>
+        </is>
+      </c>
+      <c r="T146" t="n">
+        <v>4.32</v>
+      </c>
+      <c r="U146" t="inlineStr">
+        <is>
+          <t>21/12/2023 14:36</t>
+        </is>
+      </c>
+      <c r="V146" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/serbia/super-liga/novi-pazar-spartak-subotica/dtRibpGh/</t>
         </is>
       </c>
     </row>

</xml_diff>